<commit_message>
Added wallet balance for gov. participants
</commit_message>
<xml_diff>
--- a/dataset/traders_hyperliquid.xlsx
+++ b/dataset/traders_hyperliquid.xlsx
@@ -602,15 +602,15 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1242884.615012</v>
+        <v>1268770.340617</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2024-01-14</t>
+          <t>2024-01-18</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -9863,7 +9863,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>0xca93c1c564bf5a4e8dcca65ce80fbdf66990927d</t>
+          <t>0xa68c548f3acd23a7fe3e867cc47f302559794419</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -9885,7 +9885,7 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>2023-12-04</t>
+          <t>2023-12-20</t>
         </is>
       </c>
       <c r="H270" t="inlineStr"/>
@@ -9933,7 +9933,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>0xa68c548f3acd23a7fe3e867cc47f302559794419</t>
+          <t>0x10a0695b00de0ae8baf9bb417df00efbbdd6636c</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -9951,11 +9951,11 @@
       </c>
       <c r="E272" t="inlineStr"/>
       <c r="F272" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>2023-12-20</t>
+          <t>2023-10-15</t>
         </is>
       </c>
       <c r="H272" t="inlineStr"/>
@@ -9968,7 +9968,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>0xf19a8f29096ced385abb7c4930548121c97c8c40</t>
+          <t>0xca93c1c564bf5a4e8dcca65ce80fbdf66990927d</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -9986,11 +9986,11 @@
       </c>
       <c r="E273" t="inlineStr"/>
       <c r="F273" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>2023-12-09</t>
+          <t>2023-12-04</t>
         </is>
       </c>
       <c r="H273" t="inlineStr"/>
@@ -10038,7 +10038,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>0x10a0695b00de0ae8baf9bb417df00efbbdd6636c</t>
+          <t>0xf19a8f29096ced385abb7c4930548121c97c8c40</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -10056,11 +10056,11 @@
       </c>
       <c r="E275" t="inlineStr"/>
       <c r="F275" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>2023-10-15</t>
+          <t>2023-12-09</t>
         </is>
       </c>
       <c r="H275" t="inlineStr"/>
@@ -16863,7 +16863,7 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>0x0c5d40f98a99822aee477f14666967ddea13ac54</t>
+          <t>0xb5fb748ec3e019a7ed4f6f701158bc23fa3a2626</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
@@ -16885,7 +16885,7 @@
       </c>
       <c r="G470" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>2023-12-18</t>
         </is>
       </c>
       <c r="H470" t="inlineStr"/>
@@ -16898,7 +16898,7 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>0x67f72412a592d066a2e688e62664116deabeab29</t>
+          <t>0x0c5d40f98a99822aee477f14666967ddea13ac54</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
@@ -16920,7 +16920,7 @@
       </c>
       <c r="G471" t="inlineStr">
         <is>
-          <t>2023-11-29</t>
+          <t>2023-11-01</t>
         </is>
       </c>
       <c r="H471" t="inlineStr"/>
@@ -16933,7 +16933,7 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>0xb5fb748ec3e019a7ed4f6f701158bc23fa3a2626</t>
+          <t>0x6caa8d654ef4cd907a2c498414ac9dc46106f1c2</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
@@ -16955,7 +16955,7 @@
       </c>
       <c r="G472" t="inlineStr">
         <is>
-          <t>2023-12-18</t>
+          <t>2023-08-26</t>
         </is>
       </c>
       <c r="H472" t="inlineStr"/>
@@ -16968,7 +16968,7 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>0xa4b5e04c196d864ab8534e1c302562dd9dbf1d06</t>
+          <t>0x6cc3a15e11f7c3af621b1af89c39a9608b5a5065</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
@@ -16990,7 +16990,7 @@
       </c>
       <c r="G473" t="inlineStr">
         <is>
-          <t>2023-12-06</t>
+          <t>2023-08-24</t>
         </is>
       </c>
       <c r="H473" t="inlineStr"/>
@@ -17003,7 +17003,7 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>0x2d4efbe0a82787669e9284c5f0fe160c4768e573</t>
+          <t>0xcd81917ff5313d02d7da3d47a9afcd3f635c36e3</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
@@ -17025,7 +17025,7 @@
       </c>
       <c r="G474" t="inlineStr">
         <is>
-          <t>2023-12-06</t>
+          <t>2023-12-11</t>
         </is>
       </c>
       <c r="H474" t="inlineStr"/>
@@ -17038,7 +17038,7 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>0x9425d93fa42eb85fb4ec02e5e92e63c4251eb45f</t>
+          <t>0x67f72412a592d066a2e688e62664116deabeab29</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
@@ -17060,7 +17060,7 @@
       </c>
       <c r="G475" t="inlineStr">
         <is>
-          <t>2023-12-08</t>
+          <t>2023-11-29</t>
         </is>
       </c>
       <c r="H475" t="inlineStr"/>
@@ -17073,7 +17073,7 @@
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>0x6caa8d654ef4cd907a2c498414ac9dc46106f1c2</t>
+          <t>0x27eab7d3ce4c84b9afb0324deb7c56bd72fc2fa0</t>
         </is>
       </c>
       <c r="B476" t="inlineStr">
@@ -17095,7 +17095,7 @@
       </c>
       <c r="G476" t="inlineStr">
         <is>
-          <t>2023-08-26</t>
+          <t>2023-12-15</t>
         </is>
       </c>
       <c r="H476" t="inlineStr"/>
@@ -17108,7 +17108,7 @@
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>0xcd81917ff5313d02d7da3d47a9afcd3f635c36e3</t>
+          <t>0x9425d93fa42eb85fb4ec02e5e92e63c4251eb45f</t>
         </is>
       </c>
       <c r="B477" t="inlineStr">
@@ -17130,7 +17130,7 @@
       </c>
       <c r="G477" t="inlineStr">
         <is>
-          <t>2023-12-11</t>
+          <t>2023-12-08</t>
         </is>
       </c>
       <c r="H477" t="inlineStr"/>
@@ -17143,7 +17143,7 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>0x6cc3a15e11f7c3af621b1af89c39a9608b5a5065</t>
+          <t>0xa4b5e04c196d864ab8534e1c302562dd9dbf1d06</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
@@ -17165,7 +17165,7 @@
       </c>
       <c r="G478" t="inlineStr">
         <is>
-          <t>2023-08-24</t>
+          <t>2023-12-06</t>
         </is>
       </c>
       <c r="H478" t="inlineStr"/>
@@ -17178,7 +17178,7 @@
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>0x27eab7d3ce4c84b9afb0324deb7c56bd72fc2fa0</t>
+          <t>0x2d4efbe0a82787669e9284c5f0fe160c4768e573</t>
         </is>
       </c>
       <c r="B479" t="inlineStr">
@@ -17200,7 +17200,7 @@
       </c>
       <c r="G479" t="inlineStr">
         <is>
-          <t>2023-12-15</t>
+          <t>2023-12-06</t>
         </is>
       </c>
       <c r="H479" t="inlineStr"/>
@@ -20818,7 +20818,7 @@
     <row r="583">
       <c r="A583" t="inlineStr">
         <is>
-          <t>0x65493af0bb888451c652d76f8725f392af4abedd</t>
+          <t>0x9c1915f821912f5bbcbbd07ef92cee9cf28068d4</t>
         </is>
       </c>
       <c r="B583" t="inlineStr">
@@ -20840,7 +20840,7 @@
       </c>
       <c r="G583" t="inlineStr">
         <is>
-          <t>2023-11-12</t>
+          <t>2023-08-22</t>
         </is>
       </c>
       <c r="H583" t="inlineStr"/>
@@ -20923,7 +20923,7 @@
     <row r="586">
       <c r="A586" t="inlineStr">
         <is>
-          <t>0x9c1915f821912f5bbcbbd07ef92cee9cf28068d4</t>
+          <t>0x7be11f3b8b730d413c8e64b73bd1c9557f9a2317</t>
         </is>
       </c>
       <c r="B586" t="inlineStr">
@@ -20945,7 +20945,7 @@
       </c>
       <c r="G586" t="inlineStr">
         <is>
-          <t>2023-08-22</t>
+          <t>2023-12-06</t>
         </is>
       </c>
       <c r="H586" t="inlineStr"/>
@@ -20958,7 +20958,7 @@
     <row r="587">
       <c r="A587" t="inlineStr">
         <is>
-          <t>0x7be11f3b8b730d413c8e64b73bd1c9557f9a2317</t>
+          <t>0x65493af0bb888451c652d76f8725f392af4abedd</t>
         </is>
       </c>
       <c r="B587" t="inlineStr">
@@ -20980,7 +20980,7 @@
       </c>
       <c r="G587" t="inlineStr">
         <is>
-          <t>2023-12-06</t>
+          <t>2023-11-12</t>
         </is>
       </c>
       <c r="H587" t="inlineStr"/>
@@ -22673,7 +22673,7 @@
     <row r="636">
       <c r="A636" t="inlineStr">
         <is>
-          <t>0xf944a43040980ec2d08c10cac737cd5c206db3e5</t>
+          <t>0x27af3d4795469123f94e5c0797049a79d7728d6e</t>
         </is>
       </c>
       <c r="B636" t="inlineStr">
@@ -22691,11 +22691,11 @@
       </c>
       <c r="E636" t="inlineStr"/>
       <c r="F636" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G636" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>2023-12-09</t>
         </is>
       </c>
       <c r="H636" t="inlineStr"/>
@@ -22743,7 +22743,7 @@
     <row r="638">
       <c r="A638" t="inlineStr">
         <is>
-          <t>0x0f6a1344927f794b8976713eb673c1a5cacf27e8</t>
+          <t>0xf944a43040980ec2d08c10cac737cd5c206db3e5</t>
         </is>
       </c>
       <c r="B638" t="inlineStr">
@@ -22761,11 +22761,11 @@
       </c>
       <c r="E638" t="inlineStr"/>
       <c r="F638" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G638" t="inlineStr">
         <is>
-          <t>2023-08-21</t>
+          <t>2023-11-09</t>
         </is>
       </c>
       <c r="H638" t="inlineStr"/>
@@ -22778,7 +22778,7 @@
     <row r="639">
       <c r="A639" t="inlineStr">
         <is>
-          <t>0x27af3d4795469123f94e5c0797049a79d7728d6e</t>
+          <t>0x0f6a1344927f794b8976713eb673c1a5cacf27e8</t>
         </is>
       </c>
       <c r="B639" t="inlineStr">
@@ -22796,11 +22796,11 @@
       </c>
       <c r="E639" t="inlineStr"/>
       <c r="F639" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G639" t="inlineStr">
         <is>
-          <t>2023-12-09</t>
+          <t>2023-08-21</t>
         </is>
       </c>
       <c r="H639" t="inlineStr"/>
@@ -25508,7 +25508,7 @@
     <row r="717">
       <c r="A717" t="inlineStr">
         <is>
-          <t>0x0e17d43b80eb87a5edaac7fc4c672feca2bba85a</t>
+          <t>0xe02f15fc13331041a23141ae85d490366d4d4e8d</t>
         </is>
       </c>
       <c r="B717" t="inlineStr">
@@ -25526,11 +25526,11 @@
       </c>
       <c r="E717" t="inlineStr"/>
       <c r="F717" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G717" t="inlineStr">
         <is>
-          <t>2023-11-29</t>
+          <t>2023-12-17</t>
         </is>
       </c>
       <c r="H717" t="inlineStr"/>
@@ -25543,7 +25543,7 @@
     <row r="718">
       <c r="A718" t="inlineStr">
         <is>
-          <t>0xe02f15fc13331041a23141ae85d490366d4d4e8d</t>
+          <t>0x0e17d43b80eb87a5edaac7fc4c672feca2bba85a</t>
         </is>
       </c>
       <c r="B718" t="inlineStr">
@@ -25561,11 +25561,11 @@
       </c>
       <c r="E718" t="inlineStr"/>
       <c r="F718" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G718" t="inlineStr">
         <is>
-          <t>2023-12-17</t>
+          <t>2023-11-29</t>
         </is>
       </c>
       <c r="H718" t="inlineStr"/>
@@ -31668,7 +31668,7 @@
     <row r="893">
       <c r="A893" t="inlineStr">
         <is>
-          <t>0x9b8f382e009988aa62c2aa3cd719e7fd5fd032d7</t>
+          <t>0xf65d6c4e7395bb29eab24589c8bb8a55ad47222c</t>
         </is>
       </c>
       <c r="B893" t="inlineStr">
@@ -31703,7 +31703,7 @@
     <row r="894">
       <c r="A894" t="inlineStr">
         <is>
-          <t>0xf65d6c4e7395bb29eab24589c8bb8a55ad47222c</t>
+          <t>0x11e658214247565568d6a0c0fd8e54c58f0b27d0</t>
         </is>
       </c>
       <c r="B894" t="inlineStr">
@@ -31725,7 +31725,7 @@
       </c>
       <c r="G894" t="inlineStr">
         <is>
-          <t>2023-11-28</t>
+          <t>2023-08-21</t>
         </is>
       </c>
       <c r="H894" t="inlineStr"/>
@@ -31738,7 +31738,7 @@
     <row r="895">
       <c r="A895" t="inlineStr">
         <is>
-          <t>0x48e87c81a1aece2a39b4facd8efdc3fcd63c636c</t>
+          <t>0x9b8f382e009988aa62c2aa3cd719e7fd5fd032d7</t>
         </is>
       </c>
       <c r="B895" t="inlineStr">
@@ -31760,7 +31760,7 @@
       </c>
       <c r="G895" t="inlineStr">
         <is>
-          <t>2023-12-06</t>
+          <t>2023-11-28</t>
         </is>
       </c>
       <c r="H895" t="inlineStr"/>
@@ -31808,7 +31808,7 @@
     <row r="897">
       <c r="A897" t="inlineStr">
         <is>
-          <t>0x11e658214247565568d6a0c0fd8e54c58f0b27d0</t>
+          <t>0x48e87c81a1aece2a39b4facd8efdc3fcd63c636c</t>
         </is>
       </c>
       <c r="B897" t="inlineStr">
@@ -31830,7 +31830,7 @@
       </c>
       <c r="G897" t="inlineStr">
         <is>
-          <t>2023-08-21</t>
+          <t>2023-12-06</t>
         </is>
       </c>
       <c r="H897" t="inlineStr"/>
@@ -34048,7 +34048,7 @@
     <row r="961">
       <c r="A961" t="inlineStr">
         <is>
-          <t>0x76c2b5dc369a7711e19760fb2220c981b3cc6d9e</t>
+          <t>0x000d4eeee8e0e254a6a46ee1ab6d6296ba0db1da</t>
         </is>
       </c>
       <c r="B961" t="inlineStr">
@@ -34070,7 +34070,7 @@
       </c>
       <c r="G961" t="inlineStr">
         <is>
-          <t>2023-12-08</t>
+          <t>2023-12-17</t>
         </is>
       </c>
       <c r="H961" t="inlineStr"/>
@@ -34083,7 +34083,7 @@
     <row r="962">
       <c r="A962" t="inlineStr">
         <is>
-          <t>0x4b1f4a57e0a6ef42cb38a0eba624ed87980e0002</t>
+          <t>0x65f946b64bd609259e2192bdc1bb9e80caf7c855</t>
         </is>
       </c>
       <c r="B962" t="inlineStr">
@@ -34101,11 +34101,11 @@
       </c>
       <c r="E962" t="inlineStr"/>
       <c r="F962" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G962" t="inlineStr">
         <is>
-          <t>2023-12-09</t>
+          <t>2023-09-15</t>
         </is>
       </c>
       <c r="H962" t="inlineStr"/>
@@ -34118,7 +34118,7 @@
     <row r="963">
       <c r="A963" t="inlineStr">
         <is>
-          <t>0xb90493d0876734f77a088538e9d49065f9de4d30</t>
+          <t>0xd603a49886c9b500f96c0d798aed10068d73bf7c</t>
         </is>
       </c>
       <c r="B963" t="inlineStr">
@@ -34136,11 +34136,11 @@
       </c>
       <c r="E963" t="inlineStr"/>
       <c r="F963" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G963" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>2023-11-26</t>
         </is>
       </c>
       <c r="H963" t="inlineStr"/>
@@ -34153,7 +34153,7 @@
     <row r="964">
       <c r="A964" t="inlineStr">
         <is>
-          <t>0x77ad5d16ca853e84b9b07ee5359d706d00d65f8d</t>
+          <t>0x06bbb24d6b811fd15c78815060f562df3324eed5</t>
         </is>
       </c>
       <c r="B964" t="inlineStr">
@@ -34171,11 +34171,11 @@
       </c>
       <c r="E964" t="inlineStr"/>
       <c r="F964" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G964" t="inlineStr">
         <is>
-          <t>2023-10-23</t>
+          <t>2023-12-06</t>
         </is>
       </c>
       <c r="H964" t="inlineStr"/>
@@ -34188,7 +34188,7 @@
     <row r="965">
       <c r="A965" t="inlineStr">
         <is>
-          <t>0xc1a9bc22cc31ab64a78421befa10c359a1417ce3</t>
+          <t>0xb90493d0876734f77a088538e9d49065f9de4d30</t>
         </is>
       </c>
       <c r="B965" t="inlineStr">
@@ -34210,7 +34210,7 @@
       </c>
       <c r="G965" t="inlineStr">
         <is>
-          <t>2023-08-21</t>
+          <t>2023-11-10</t>
         </is>
       </c>
       <c r="H965" t="inlineStr"/>
@@ -34223,7 +34223,7 @@
     <row r="966">
       <c r="A966" t="inlineStr">
         <is>
-          <t>0xd603a49886c9b500f96c0d798aed10068d73bf7c</t>
+          <t>0x4b1f4a57e0a6ef42cb38a0eba624ed87980e0002</t>
         </is>
       </c>
       <c r="B966" t="inlineStr">
@@ -34241,11 +34241,11 @@
       </c>
       <c r="E966" t="inlineStr"/>
       <c r="F966" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G966" t="inlineStr">
         <is>
-          <t>2023-11-26</t>
+          <t>2023-12-09</t>
         </is>
       </c>
       <c r="H966" t="inlineStr"/>
@@ -34258,7 +34258,7 @@
     <row r="967">
       <c r="A967" t="inlineStr">
         <is>
-          <t>0x441c8cbe1aa06beea4c84cfff5e12753f37822fb</t>
+          <t>0x75331ebbe0b00b97cab532384f13c9b479f074ec</t>
         </is>
       </c>
       <c r="B967" t="inlineStr">
@@ -34280,7 +34280,7 @@
       </c>
       <c r="G967" t="inlineStr">
         <is>
-          <t>2023-12-14</t>
+          <t>2023-12-04</t>
         </is>
       </c>
       <c r="H967" t="inlineStr"/>
@@ -34293,7 +34293,7 @@
     <row r="968">
       <c r="A968" t="inlineStr">
         <is>
-          <t>0x75331ebbe0b00b97cab532384f13c9b479f074ec</t>
+          <t>0xc1a9bc22cc31ab64a78421befa10c359a1417ce3</t>
         </is>
       </c>
       <c r="B968" t="inlineStr">
@@ -34315,7 +34315,7 @@
       </c>
       <c r="G968" t="inlineStr">
         <is>
-          <t>2023-12-04</t>
+          <t>2023-08-21</t>
         </is>
       </c>
       <c r="H968" t="inlineStr"/>
@@ -34328,7 +34328,7 @@
     <row r="969">
       <c r="A969" t="inlineStr">
         <is>
-          <t>0x65f946b64bd609259e2192bdc1bb9e80caf7c855</t>
+          <t>0x77ad5d16ca853e84b9b07ee5359d706d00d65f8d</t>
         </is>
       </c>
       <c r="B969" t="inlineStr">
@@ -34346,11 +34346,11 @@
       </c>
       <c r="E969" t="inlineStr"/>
       <c r="F969" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G969" t="inlineStr">
         <is>
-          <t>2023-09-15</t>
+          <t>2023-10-23</t>
         </is>
       </c>
       <c r="H969" t="inlineStr"/>
@@ -34363,7 +34363,7 @@
     <row r="970">
       <c r="A970" t="inlineStr">
         <is>
-          <t>0x06bbb24d6b811fd15c78815060f562df3324eed5</t>
+          <t>0x441c8cbe1aa06beea4c84cfff5e12753f37822fb</t>
         </is>
       </c>
       <c r="B970" t="inlineStr">
@@ -34385,7 +34385,7 @@
       </c>
       <c r="G970" t="inlineStr">
         <is>
-          <t>2023-12-06</t>
+          <t>2023-12-14</t>
         </is>
       </c>
       <c r="H970" t="inlineStr"/>
@@ -34398,7 +34398,7 @@
     <row r="971">
       <c r="A971" t="inlineStr">
         <is>
-          <t>0x000d4eeee8e0e254a6a46ee1ab6d6296ba0db1da</t>
+          <t>0x325c08a558ff02f244f31ba1e87bf3c1b1c08f45</t>
         </is>
       </c>
       <c r="B971" t="inlineStr">
@@ -34420,7 +34420,7 @@
       </c>
       <c r="G971" t="inlineStr">
         <is>
-          <t>2023-12-17</t>
+          <t>2023-11-24</t>
         </is>
       </c>
       <c r="H971" t="inlineStr"/>
@@ -34433,7 +34433,7 @@
     <row r="972">
       <c r="A972" t="inlineStr">
         <is>
-          <t>0x325c08a558ff02f244f31ba1e87bf3c1b1c08f45</t>
+          <t>0x76c2b5dc369a7711e19760fb2220c981b3cc6d9e</t>
         </is>
       </c>
       <c r="B972" t="inlineStr">
@@ -34455,7 +34455,7 @@
       </c>
       <c r="G972" t="inlineStr">
         <is>
-          <t>2023-11-24</t>
+          <t>2023-12-08</t>
         </is>
       </c>
       <c r="H972" t="inlineStr"/>
@@ -38808,7 +38808,7 @@
     <row r="1097">
       <c r="A1097" t="inlineStr">
         <is>
-          <t>0x3b1b211b3fce0d1ee9f5e1afeecadeb98378d0b0</t>
+          <t>0x4461d605a73f4f0ea2d52b89c8b36ec78d7f56fd</t>
         </is>
       </c>
       <c r="B1097" t="inlineStr">
@@ -38826,11 +38826,11 @@
       </c>
       <c r="E1097" t="inlineStr"/>
       <c r="F1097" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G1097" t="inlineStr">
         <is>
-          <t>2023-11-22</t>
+          <t>2023-12-14</t>
         </is>
       </c>
       <c r="H1097" t="inlineStr"/>
@@ -38843,7 +38843,7 @@
     <row r="1098">
       <c r="A1098" t="inlineStr">
         <is>
-          <t>0x4461d605a73f4f0ea2d52b89c8b36ec78d7f56fd</t>
+          <t>0x3b1b211b3fce0d1ee9f5e1afeecadeb98378d0b0</t>
         </is>
       </c>
       <c r="B1098" t="inlineStr">
@@ -38861,11 +38861,11 @@
       </c>
       <c r="E1098" t="inlineStr"/>
       <c r="F1098" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G1098" t="inlineStr">
         <is>
-          <t>2023-12-14</t>
+          <t>2023-11-22</t>
         </is>
       </c>
       <c r="H1098" t="inlineStr"/>
@@ -40908,7 +40908,7 @@
     <row r="1157">
       <c r="A1157" t="inlineStr">
         <is>
-          <t>0xdb93321a059456bc61df08c80468ef803810abc5</t>
+          <t>0x8ff2c6dda9a3f2d88171b4d6a0cb81915ac53f66</t>
         </is>
       </c>
       <c r="B1157" t="inlineStr">
@@ -40926,11 +40926,11 @@
       </c>
       <c r="E1157" t="inlineStr"/>
       <c r="F1157" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G1157" t="inlineStr">
         <is>
-          <t>2023-11-20</t>
+          <t>2023-11-27</t>
         </is>
       </c>
       <c r="H1157" t="inlineStr"/>
@@ -41013,7 +41013,7 @@
     <row r="1160">
       <c r="A1160" t="inlineStr">
         <is>
-          <t>0x9224bbb4e0fbe2f2f8fab55debc41eb21fdfb804</t>
+          <t>0xdb93321a059456bc61df08c80468ef803810abc5</t>
         </is>
       </c>
       <c r="B1160" t="inlineStr">
@@ -41031,11 +41031,11 @@
       </c>
       <c r="E1160" t="inlineStr"/>
       <c r="F1160" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G1160" t="inlineStr">
         <is>
-          <t>2023-12-20</t>
+          <t>2023-11-20</t>
         </is>
       </c>
       <c r="H1160" t="inlineStr"/>
@@ -41048,7 +41048,7 @@
     <row r="1161">
       <c r="A1161" t="inlineStr">
         <is>
-          <t>0x8ff2c6dda9a3f2d88171b4d6a0cb81915ac53f66</t>
+          <t>0x9224bbb4e0fbe2f2f8fab55debc41eb21fdfb804</t>
         </is>
       </c>
       <c r="B1161" t="inlineStr">
@@ -41066,11 +41066,11 @@
       </c>
       <c r="E1161" t="inlineStr"/>
       <c r="F1161" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G1161" t="inlineStr">
         <is>
-          <t>2023-11-27</t>
+          <t>2023-12-20</t>
         </is>
       </c>
       <c r="H1161" t="inlineStr"/>
@@ -44863,7 +44863,7 @@
     <row r="1270">
       <c r="A1270" t="inlineStr">
         <is>
-          <t>0x7eb12f04effc4901d7520e4ebd62de512743feca</t>
+          <t>0xcdec10792b5793c7670f9f3667370c74b0de2353</t>
         </is>
       </c>
       <c r="B1270" t="inlineStr">
@@ -44885,7 +44885,7 @@
       </c>
       <c r="G1270" t="inlineStr">
         <is>
-          <t>2023-12-10</t>
+          <t>2023-12-20</t>
         </is>
       </c>
       <c r="H1270" t="inlineStr"/>
@@ -44898,7 +44898,7 @@
     <row r="1271">
       <c r="A1271" t="inlineStr">
         <is>
-          <t>0xcdec10792b5793c7670f9f3667370c74b0de2353</t>
+          <t>0x7eb12f04effc4901d7520e4ebd62de512743feca</t>
         </is>
       </c>
       <c r="B1271" t="inlineStr">
@@ -44920,7 +44920,7 @@
       </c>
       <c r="G1271" t="inlineStr">
         <is>
-          <t>2023-12-20</t>
+          <t>2023-12-10</t>
         </is>
       </c>
       <c r="H1271" t="inlineStr"/>
@@ -50988,7 +50988,7 @@
     <row r="1445">
       <c r="A1445" t="inlineStr">
         <is>
-          <t>0xb5cf6c54887e03716d1c6ebdb0e9f49d0c3bed6a</t>
+          <t>0x2af451e8ad601d26b11c882c4b2a558221e74587</t>
         </is>
       </c>
       <c r="B1445" t="inlineStr">
@@ -51006,11 +51006,11 @@
       </c>
       <c r="E1445" t="inlineStr"/>
       <c r="F1445" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G1445" t="inlineStr">
         <is>
-          <t>2023-12-07</t>
+          <t>2023-12-08</t>
         </is>
       </c>
       <c r="H1445" t="inlineStr"/>
@@ -51023,7 +51023,7 @@
     <row r="1446">
       <c r="A1446" t="inlineStr">
         <is>
-          <t>0x2af451e8ad601d26b11c882c4b2a558221e74587</t>
+          <t>0x547c8d938b98cd17ab7c653a0d98cca80eabb876</t>
         </is>
       </c>
       <c r="B1446" t="inlineStr">
@@ -51041,11 +51041,11 @@
       </c>
       <c r="E1446" t="inlineStr"/>
       <c r="F1446" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G1446" t="inlineStr">
         <is>
-          <t>2023-12-08</t>
+          <t>2023-12-07</t>
         </is>
       </c>
       <c r="H1446" t="inlineStr"/>
@@ -51058,7 +51058,7 @@
     <row r="1447">
       <c r="A1447" t="inlineStr">
         <is>
-          <t>0x0a44bfd056cac5518946b05d0a57bc3011073e57</t>
+          <t>0xb5cf6c54887e03716d1c6ebdb0e9f49d0c3bed6a</t>
         </is>
       </c>
       <c r="B1447" t="inlineStr">
@@ -51076,11 +51076,11 @@
       </c>
       <c r="E1447" t="inlineStr"/>
       <c r="F1447" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G1447" t="inlineStr">
         <is>
-          <t>2023-12-18</t>
+          <t>2023-12-07</t>
         </is>
       </c>
       <c r="H1447" t="inlineStr"/>
@@ -51093,7 +51093,7 @@
     <row r="1448">
       <c r="A1448" t="inlineStr">
         <is>
-          <t>0x547c8d938b98cd17ab7c653a0d98cca80eabb876</t>
+          <t>0x0a44bfd056cac5518946b05d0a57bc3011073e57</t>
         </is>
       </c>
       <c r="B1448" t="inlineStr">
@@ -51111,11 +51111,11 @@
       </c>
       <c r="E1448" t="inlineStr"/>
       <c r="F1448" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G1448" t="inlineStr">
         <is>
-          <t>2023-12-07</t>
+          <t>2023-12-18</t>
         </is>
       </c>
       <c r="H1448" t="inlineStr"/>
@@ -53333,7 +53333,7 @@
     <row r="1512">
       <c r="A1512" t="inlineStr">
         <is>
-          <t>0x8476b6a8aa0b4037e69e79f116f662aa0096b0c0</t>
+          <t>0xe00163c3921c6b16afce692a398415e8253db99c</t>
         </is>
       </c>
       <c r="B1512" t="inlineStr">
@@ -53355,7 +53355,7 @@
       </c>
       <c r="G1512" t="inlineStr">
         <is>
-          <t>2023-11-26</t>
+          <t>2023-12-02</t>
         </is>
       </c>
       <c r="H1512" t="inlineStr"/>
@@ -53403,7 +53403,7 @@
     <row r="1514">
       <c r="A1514" t="inlineStr">
         <is>
-          <t>0xe00163c3921c6b16afce692a398415e8253db99c</t>
+          <t>0x8476b6a8aa0b4037e69e79f116f662aa0096b0c0</t>
         </is>
       </c>
       <c r="B1514" t="inlineStr">
@@ -53425,7 +53425,7 @@
       </c>
       <c r="G1514" t="inlineStr">
         <is>
-          <t>2023-12-02</t>
+          <t>2023-11-26</t>
         </is>
       </c>
       <c r="H1514" t="inlineStr"/>

</xml_diff>